<commit_message>
added filtering for 40017-B
</commit_message>
<xml_diff>
--- a/samples/TD08082019.xlsx
+++ b/samples/TD08082019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\China Life Franklin Asset Management\IT - Documents\General\20190816 Trade file conversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\AppData\Local\Programs\Git\git\tradefeed_cmbhk\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{C93BA185-5A3A-48EF-8582-8502BA37C5E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{683522D3-84AB-45E4-94F6-1C25B3261F08}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E98A56-4039-45FA-A389-7E697A725CC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t9208531" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Citic Future ON 08/08/19</t>
   </si>
@@ -138,6 +138,12 @@
   <si>
     <t>China Life Franklin - CMFHK China Life Franklin Global Fixed Income Opportunities SP</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>40017-B</t>
   </si>
 </sst>
 </file>
@@ -1104,15 +1110,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
@@ -1127,114 +1133,118 @@
     <col min="16" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="20" width="15" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>1.625</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>1.717616</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>43685</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>43692</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>1000000</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>99.15234375</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
@@ -1245,55 +1255,58 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="1">
+      <c r="S5" s="1">
         <v>0</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="3">
         <v>991523.44</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>4.875</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>3.4582329999999999</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>43685</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>43689</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>500000</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>102.95</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -1304,55 +1317,58 @@
       <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
         <v>7718.75</v>
       </c>
-      <c r="S6" s="3">
+      <c r="T6" s="3">
         <v>522468.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>10.5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>8.5514390000000002</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>43685</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>43689</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>1000000</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>104.375</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
       </c>
       <c r="M7" s="1">
         <v>0</v>
@@ -1363,16 +1379,19 @@
       <c r="O7" s="1">
         <v>0</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>46958.33</v>
       </c>
-      <c r="S7" s="3">
+      <c r="T7" s="3">
         <v>1090708.33</v>
       </c>
     </row>
@@ -1383,15 +1402,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3ABBA213F535143A2153FAFFCD4B404" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de5c07bc042d9b8335c64ae2844aa26e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56ce6572-a240-4cd6-8225-c99230995deb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a3b6e2b5c3108d7449c3295a83331ef" ns2:_="">
     <xsd:import namespace="56ce6572-a240-4cd6-8225-c99230995deb"/>
@@ -1555,6 +1565,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1562,14 +1581,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE897917-9B72-489E-9E8F-BC08A110811C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82CDEFFD-4BE9-4AA8-911A-DC91A1E64EFE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1583,6 +1594,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE897917-9B72-489E-9E8F-BC08A110811C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
made changes according to Chelsea request
</commit_message>
<xml_diff>
--- a/samples/TD08082019.xlsx
+++ b/samples/TD08082019.xlsx
@@ -5,22 +5,30 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\AppData\Local\Programs\Git\git\tradefeed_cmbhk\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\AppData\Local\Programs\Git\git\tradefeed_cmbhk\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E98A56-4039-45FA-A389-7E697A725CC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BB8C02-AC73-49FF-9D2F-0BFFC2A3C81E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2175" windowWidth="23970" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t9208531" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Citic Future ON 08/08/19</t>
   </si>
@@ -144,6 +152,9 @@
   </si>
   <si>
     <t>40017-B</t>
+  </si>
+  <si>
+    <t>Principal</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1132,22 +1143,23 @@
     <col min="12" max="15" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="19" width="12.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -1203,13 +1215,16 @@
         <v>17</v>
       </c>
       <c r="S4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1264,14 +1279,18 @@
       <c r="R5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="3">
+        <f>U5-T5</f>
+        <v>991523.44</v>
+      </c>
+      <c r="T5" s="1">
         <v>0</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="3">
         <v>991523.44</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -1326,14 +1345,18 @@
       <c r="R6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="3">
+        <f t="shared" ref="S6:S7" si="0">U6-T6</f>
+        <v>514750</v>
+      </c>
+      <c r="T6" s="1">
         <v>7718.75</v>
       </c>
-      <c r="T6" s="3">
+      <c r="U6" s="3">
         <v>522468.75</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -1388,10 +1411,14 @@
       <c r="R7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="3">
+        <f t="shared" si="0"/>
+        <v>1043750.0000000001</v>
+      </c>
+      <c r="T7" s="1">
         <v>46958.33</v>
       </c>
-      <c r="T7" s="3">
+      <c r="U7" s="3">
         <v>1090708.33</v>
       </c>
     </row>
@@ -1402,6 +1429,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3ABBA213F535143A2153FAFFCD4B404" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="de5c07bc042d9b8335c64ae2844aa26e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56ce6572-a240-4cd6-8225-c99230995deb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6a3b6e2b5c3108d7449c3295a83331ef" ns2:_="">
     <xsd:import namespace="56ce6572-a240-4cd6-8225-c99230995deb"/>
@@ -1565,15 +1601,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1581,6 +1608,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE897917-9B72-489E-9E8F-BC08A110811C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82CDEFFD-4BE9-4AA8-911A-DC91A1E64EFE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1594,14 +1629,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE897917-9B72-489E-9E8F-BC08A110811C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>